<commit_message>
DC motor model change.
</commit_message>
<xml_diff>
--- a/Dokumentacja/Elementy.xlsx
+++ b/Dokumentacja/Elementy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcel.garczyk\Desktop\Dokumentacja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8A455C-39D2-4193-8372-3299DB224E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5AAAB9-E0F8-408A-BD9C-802ADD829424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3597A509-DA09-4DA2-982F-86233DA0E059}"/>
+    <workbookView xWindow="28680" yWindow="4575" windowWidth="20730" windowHeight="11160" xr2:uid="{3597A509-DA09-4DA2-982F-86233DA0E059}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Rock 4 C+ Radxa RS114CP-D4 4 GB 6 x 1.5 GHz, 1.0 GHz</t>
   </si>
   <si>
-    <t>Silnik z przekładnią 6V 100RPM + enkoder</t>
-  </si>
-  <si>
     <t>Cytron MDD20A - dwukanałowy sterownik silników DC 30V/20A</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>99:1 METAL GEARMOTOR 25DX69L LP 6V 48 CPPOLOLU</t>
   </si>
 </sst>
 </file>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE234BC4-669A-426C-8618-8A645FB96B7D}">
   <dimension ref="F4:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +645,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H7" s="9">
         <v>4</v>
@@ -659,7 +659,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H8" s="9">
         <v>2</v>
@@ -673,7 +673,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H9" s="9">
         <v>1</v>
@@ -682,7 +682,7 @@
         <v>225</v>
       </c>
       <c r="P9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="6:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -690,7 +690,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H10" s="9">
         <v>2</v>
@@ -704,7 +704,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="9">
         <v>1</v>
@@ -718,7 +718,7 @@
         <v>7</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H12" s="9">
         <v>1</v>
@@ -732,7 +732,7 @@
         <v>8</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="9">
         <v>1</v>
@@ -746,7 +746,7 @@
         <v>9</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" s="9">
         <v>3</v>
@@ -760,7 +760,7 @@
         <v>10</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" s="9">
         <v>1</v>
@@ -774,7 +774,7 @@
         <v>11</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H16" s="7">
         <v>4</v>
@@ -788,7 +788,7 @@
         <v>12</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H17" s="9">
         <v>1</v>
@@ -802,7 +802,7 @@
         <v>13</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H18" s="9">
         <v>1</v>
@@ -816,7 +816,7 @@
         <v>14</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="9">
         <v>1</v>
@@ -830,7 +830,7 @@
         <v>15</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H20" s="9">
         <v>1</v>
@@ -844,18 +844,18 @@
         <v>16</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="9">
         <v>3</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="6:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F22" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="14"/>
@@ -870,21 +870,21 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G6" r:id="rId1" display="https://www.conrad.pl/pl/p/rock-4-c-radxa-rs114cp-d4-4-gb-6-x-1-5-ghz-1-0-ghz-2623433.html" xr:uid="{FD6959BB-74D4-4868-B8DA-09B8D820104D}"/>
-    <hyperlink ref="G7" r:id="rId2" display="https://www.tme.eu/pl/details/pololu-4826/silniki-dc/pololu/75-1-metal-gearmotor-25dx69l-lp-6v-48-cp/" xr:uid="{3B0AB9A2-54CC-4D2B-92DE-7440974BC14F}"/>
-    <hyperlink ref="G8" r:id="rId3" display="https://botland.com.pl/sterowniki-silnikow-moduly/18881-cytron-mdd20a-dwukanalowy-sterownik-silnikow-dc-30v-20a-38515324.html" xr:uid="{85139AA3-EE20-498D-B68A-A550067F7AA8}"/>
-    <hyperlink ref="G9" r:id="rId4" display="https://botland.com.pl/czujniki-time-of-flight/15862-laserowy-czujnik-odleglosci-lidar-tfmini-s-uarti2c-12m-5903351249058.html" xr:uid="{C476B8D2-0374-4D51-ABC1-56512F489036}"/>
-    <hyperlink ref="G10" r:id="rId5" display="https://botland.com.pl/kola-z-oponami/2119-kola-dagu-wild-thumper-120x60mm-2szt-6952581600060.html" xr:uid="{ACF15833-BE65-4A53-9EDC-1E611D1F02EC}"/>
-    <hyperlink ref="G11" r:id="rId6" display="https://botland.com.pl/akumulatory-zelowe/3947-akumulator-zelowy-12v-34ah-xtreme-5900804003281.html" xr:uid="{0CAA3264-151F-4988-9CED-517D02BF1F75}"/>
-    <hyperlink ref="G12" r:id="rId7" display="https://botland.com.pl/silniki-krokowe/6424-silnik-krokowy-jk42hs40-0404-200-krokowobr-12v04a04nm-5904422334604.html" xr:uid="{59C7B0DB-5B71-4617-B28D-9B396CB83435}"/>
-    <hyperlink ref="G13" r:id="rId8" display="https://botland.com.pl/serwa-typu-micro/2314-serwo-powerhd-hd-1800a-micro-6953524540085.html" xr:uid="{B67F7777-9548-4B8A-8131-03171D12C184}"/>
-    <hyperlink ref="G14" r:id="rId9" display="https://botland.com.pl/przetwornice-step-down/8103-przetwornica-step-down-xl4015-13v-36v-5a-5904422336202.html?cd=18298825651&amp;ad=&amp;kd=&amp;gclid=CjwKCAjwm4ukBhAuEiwA0zQxk90JYCC_l7Ab2eT_qgyha9N2EWK0_HSV8O1FtmMjD5DRyCwIWTIy0hoCliQQAvD_BwE" xr:uid="{F7BC4C8B-6979-4D5D-A8EB-15901459D665}"/>
-    <hyperlink ref="G15" r:id="rId10" display="https://botland.com.pl/sterowniki-silnikow-krokowych/2660-sterownik-silnika-krokowego-a4988-reprap-czerwony-5904422359201.html" xr:uid="{407B5B7D-0C1A-42E2-BA3C-4DF722DE4C54}"/>
-    <hyperlink ref="G16" r:id="rId11" display="https://media.digikey.com/pdf/Data%20Sheets/Adafruit%20PDFs/4019_Web.pdf" xr:uid="{95EAA54C-9BE2-45C1-8C87-822998D322BC}"/>
-    <hyperlink ref="G21" r:id="rId12" display="https://allegro.pl/oferta/plexiglas-pleksiglas-8mm-na-wymiar-10696761064?fromVariant=10696761201" xr:uid="{9A077F3A-2D39-4E2F-87CC-98F40BAEB58E}"/>
-    <hyperlink ref="G17" r:id="rId13" xr:uid="{88175512-BED8-4E2A-B13E-085AF68279E4}"/>
-    <hyperlink ref="G18" r:id="rId14" xr:uid="{E5FA72C6-B412-4EF5-8308-971C6B033241}"/>
-    <hyperlink ref="G19" r:id="rId15" xr:uid="{DE1FBF7B-6474-4B07-AFF7-75488FDE3C56}"/>
-    <hyperlink ref="G20" r:id="rId16" xr:uid="{1A60FBBD-DA30-4FD2-963E-9ED000056ED4}"/>
+    <hyperlink ref="G8" r:id="rId2" display="https://botland.com.pl/sterowniki-silnikow-moduly/18881-cytron-mdd20a-dwukanalowy-sterownik-silnikow-dc-30v-20a-38515324.html" xr:uid="{85139AA3-EE20-498D-B68A-A550067F7AA8}"/>
+    <hyperlink ref="G9" r:id="rId3" display="https://botland.com.pl/czujniki-time-of-flight/15862-laserowy-czujnik-odleglosci-lidar-tfmini-s-uarti2c-12m-5903351249058.html" xr:uid="{C476B8D2-0374-4D51-ABC1-56512F489036}"/>
+    <hyperlink ref="G10" r:id="rId4" display="https://botland.com.pl/kola-z-oponami/2119-kola-dagu-wild-thumper-120x60mm-2szt-6952581600060.html" xr:uid="{ACF15833-BE65-4A53-9EDC-1E611D1F02EC}"/>
+    <hyperlink ref="G11" r:id="rId5" display="https://botland.com.pl/akumulatory-zelowe/3947-akumulator-zelowy-12v-34ah-xtreme-5900804003281.html" xr:uid="{0CAA3264-151F-4988-9CED-517D02BF1F75}"/>
+    <hyperlink ref="G12" r:id="rId6" display="https://botland.com.pl/silniki-krokowe/6424-silnik-krokowy-jk42hs40-0404-200-krokowobr-12v04a04nm-5904422334604.html" xr:uid="{59C7B0DB-5B71-4617-B28D-9B396CB83435}"/>
+    <hyperlink ref="G13" r:id="rId7" display="https://botland.com.pl/serwa-typu-micro/2314-serwo-powerhd-hd-1800a-micro-6953524540085.html" xr:uid="{B67F7777-9548-4B8A-8131-03171D12C184}"/>
+    <hyperlink ref="G14" r:id="rId8" display="https://botland.com.pl/przetwornice-step-down/8103-przetwornica-step-down-xl4015-13v-36v-5a-5904422336202.html?cd=18298825651&amp;ad=&amp;kd=&amp;gclid=CjwKCAjwm4ukBhAuEiwA0zQxk90JYCC_l7Ab2eT_qgyha9N2EWK0_HSV8O1FtmMjD5DRyCwIWTIy0hoCliQQAvD_BwE" xr:uid="{F7BC4C8B-6979-4D5D-A8EB-15901459D665}"/>
+    <hyperlink ref="G15" r:id="rId9" display="https://botland.com.pl/sterowniki-silnikow-krokowych/2660-sterownik-silnika-krokowego-a4988-reprap-czerwony-5904422359201.html" xr:uid="{407B5B7D-0C1A-42E2-BA3C-4DF722DE4C54}"/>
+    <hyperlink ref="G16" r:id="rId10" display="https://media.digikey.com/pdf/Data%20Sheets/Adafruit%20PDFs/4019_Web.pdf" xr:uid="{95EAA54C-9BE2-45C1-8C87-822998D322BC}"/>
+    <hyperlink ref="G21" r:id="rId11" display="https://allegro.pl/oferta/plexiglas-pleksiglas-8mm-na-wymiar-10696761064?fromVariant=10696761201" xr:uid="{9A077F3A-2D39-4E2F-87CC-98F40BAEB58E}"/>
+    <hyperlink ref="G17" r:id="rId12" xr:uid="{88175512-BED8-4E2A-B13E-085AF68279E4}"/>
+    <hyperlink ref="G18" r:id="rId13" xr:uid="{E5FA72C6-B412-4EF5-8308-971C6B033241}"/>
+    <hyperlink ref="G19" r:id="rId14" xr:uid="{DE1FBF7B-6474-4B07-AFF7-75488FDE3C56}"/>
+    <hyperlink ref="G20" r:id="rId15" xr:uid="{1A60FBBD-DA30-4FD2-963E-9ED000056ED4}"/>
+    <hyperlink ref="G7" r:id="rId16" display="https://www.tme.eu/en/details/pololu-4827/dc-motors/pololu/99-1-metal-gearmotor-25dx69l-lp-6v-48-cp/" xr:uid="{3B0AB9A2-54CC-4D2B-92DE-7440974BC14F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>